<commit_message>
add runtime support from MATLAB
</commit_message>
<xml_diff>
--- a/Algorithm_tester/data_autosave/real_database_comparison.xlsx
+++ b/Algorithm_tester/data_autosave/real_database_comparison.xlsx
@@ -1145,7 +1145,7 @@
         <v>0</v>
       </c>
       <c r="F30" t="n">
-        <v>449.2678642272949</v>
+        <v>473.2589721679688</v>
       </c>
       <c r="G30" t="n">
         <v>0</v>
@@ -1167,7 +1167,7 @@
         <v>0</v>
       </c>
       <c r="F31" t="n">
-        <v>455.2164673805237</v>
+        <v>507.0305585861206</v>
       </c>
       <c r="G31" t="n">
         <v>0</v>
@@ -1189,7 +1189,7 @@
         <v>0</v>
       </c>
       <c r="F32" t="n">
-        <v>470.3037738800049</v>
+        <v>672.3466515541077</v>
       </c>
       <c r="G32" t="n">
         <v>0</v>
@@ -1211,7 +1211,7 @@
         <v>0</v>
       </c>
       <c r="F33" t="n">
-        <v>524.7342586517334</v>
+        <v>727.0430326461792</v>
       </c>
       <c r="G33" t="n">
         <v>0.6964285714285714</v>
@@ -1233,7 +1233,7 @@
         <v>0</v>
       </c>
       <c r="F34" t="n">
-        <v>623.0602860450745</v>
+        <v>746.0289001464844</v>
       </c>
       <c r="G34" t="n">
         <v>1</v>
@@ -1255,7 +1255,7 @@
         <v>0</v>
       </c>
       <c r="F35" t="n">
-        <v>795.4774022102354</v>
+        <v>864.7780656814575</v>
       </c>
       <c r="G35" t="n">
         <v>1</v>
@@ -1277,7 +1277,7 @@
         <v>0</v>
       </c>
       <c r="F36" t="n">
-        <v>893.186092376709</v>
+        <v>880.8329105377197</v>
       </c>
       <c r="G36" t="n">
         <v>1</v>
@@ -2005,7 +2005,7 @@
         <v>0.5</v>
       </c>
       <c r="F68" t="n">
-        <v>83.648681640625</v>
+        <v>101.2722253799438</v>
       </c>
       <c r="G68" t="n">
         <v>0</v>
@@ -2027,7 +2027,7 @@
         <v>1</v>
       </c>
       <c r="F69" t="n">
-        <v>260.7167363166809</v>
+        <v>325.6262540817261</v>
       </c>
       <c r="G69" t="n">
         <v>0</v>
@@ -2049,7 +2049,7 @@
         <v>1</v>
       </c>
       <c r="F70" t="n">
-        <v>307.9747796058654</v>
+        <v>408.578073978424</v>
       </c>
       <c r="G70" t="n">
         <v>0.1706896551724135</v>
@@ -2071,7 +2071,7 @@
         <v>1</v>
       </c>
       <c r="F71" t="n">
-        <v>320.7621574401855</v>
+        <v>432.3427677154541</v>
       </c>
       <c r="G71" t="n">
         <v>0.3103448275862069</v>
@@ -2733,7 +2733,7 @@
         <v>0</v>
       </c>
       <c r="F100" t="n">
-        <v>7.610082626342773</v>
+        <v>9.634971618652344</v>
       </c>
       <c r="G100" t="n">
         <v>0</v>
@@ -2755,7 +2755,7 @@
         <v>0</v>
       </c>
       <c r="F101" t="n">
-        <v>8.01767110824585</v>
+        <v>11.90927028656006</v>
       </c>
       <c r="G101" t="n">
         <v>0</v>
@@ -2777,7 +2777,7 @@
         <v>0</v>
       </c>
       <c r="F102" t="n">
-        <v>15.76989889144897</v>
+        <v>20.73484659194946</v>
       </c>
       <c r="G102" t="n">
         <v>1</v>
@@ -2799,7 +2799,7 @@
         <v>0</v>
       </c>
       <c r="F103" t="n">
-        <v>18.00274848937988</v>
+        <v>42.24205017089844</v>
       </c>
       <c r="G103" t="n">
         <v>1</v>
@@ -2821,7 +2821,7 @@
         <v>0</v>
       </c>
       <c r="F104" t="n">
-        <v>43.24263334274292</v>
+        <v>74.79268312454224</v>
       </c>
       <c r="G104" t="n">
         <v>1</v>
@@ -2843,7 +2843,7 @@
         <v>0</v>
       </c>
       <c r="F105" t="n">
-        <v>70.02769708633421</v>
+        <v>101.5661597251892</v>
       </c>
       <c r="G105" t="n">
         <v>1</v>
@@ -2865,7 +2865,7 @@
         <v>0</v>
       </c>
       <c r="F106" t="n">
-        <v>74.62167739868164</v>
+        <v>112.6465797424316</v>
       </c>
       <c r="G106" t="n">
         <v>1</v>
@@ -3527,7 +3527,7 @@
         <v>0</v>
       </c>
       <c r="F135" t="n">
-        <v>199.0480422973633</v>
+        <v>333.3365917205811</v>
       </c>
       <c r="G135" t="n">
         <v>0</v>
@@ -3549,7 +3549,7 @@
         <v>0</v>
       </c>
       <c r="F136" t="n">
-        <v>216.249692440033</v>
+        <v>335.7885599136353</v>
       </c>
       <c r="G136" t="n">
         <v>0</v>
@@ -3571,7 +3571,7 @@
         <v>0</v>
       </c>
       <c r="F137" t="n">
-        <v>265.0694847106934</v>
+        <v>352.6906967163086</v>
       </c>
       <c r="G137" t="n">
         <v>0.9584627329192547</v>
@@ -3593,7 +3593,7 @@
         <v>0</v>
       </c>
       <c r="F138" t="n">
-        <v>333.5740566253662</v>
+        <v>449.8480558395386</v>
       </c>
       <c r="G138" t="n">
         <v>0.9827586206896552</v>
@@ -3615,7 +3615,7 @@
         <v>0</v>
       </c>
       <c r="F139" t="n">
-        <v>356.111466884613</v>
+        <v>468.2725667953491</v>
       </c>
       <c r="G139" t="n">
         <v>1</v>
@@ -3637,7 +3637,7 @@
         <v>0</v>
       </c>
       <c r="F140" t="n">
-        <v>399.4000911712646</v>
+        <v>545.2590465545653</v>
       </c>
       <c r="G140" t="n">
         <v>1</v>
@@ -3659,7 +3659,7 @@
         <v>0</v>
       </c>
       <c r="F141" t="n">
-        <v>411.6275310516357</v>
+        <v>584.355354309082</v>
       </c>
       <c r="G141" t="n">
         <v>1</v>
@@ -4321,7 +4321,7 @@
         <v>0</v>
       </c>
       <c r="F170" t="n">
-        <v>22.98521995544434</v>
+        <v>33.15544128417969</v>
       </c>
       <c r="G170" t="n">
         <v>0</v>
@@ -4343,7 +4343,7 @@
         <v>0</v>
       </c>
       <c r="F171" t="n">
-        <v>23.4778881072998</v>
+        <v>36.6207480430603</v>
       </c>
       <c r="G171" t="n">
         <v>0</v>
@@ -4365,7 +4365,7 @@
         <v>0</v>
       </c>
       <c r="F172" t="n">
-        <v>27.07415819168091</v>
+        <v>50.86004734039307</v>
       </c>
       <c r="G172" t="n">
         <v>0</v>
@@ -4387,7 +4387,7 @@
         <v>0</v>
       </c>
       <c r="F173" t="n">
-        <v>33.52510929107666</v>
+        <v>56.82849884033203</v>
       </c>
       <c r="G173" t="n">
         <v>0</v>
@@ -4409,7 +4409,7 @@
         <v>0</v>
       </c>
       <c r="F174" t="n">
-        <v>47.59132862091064</v>
+        <v>65.67549705505371</v>
       </c>
       <c r="G174" t="n">
         <v>0</v>
@@ -4431,7 +4431,7 @@
         <v>0</v>
       </c>
       <c r="F175" t="n">
-        <v>71.56505584716794</v>
+        <v>68.92014741897583</v>
       </c>
       <c r="G175" t="n">
         <v>0.9624999999999999</v>
@@ -4453,7 +4453,7 @@
         <v>0</v>
       </c>
       <c r="F176" t="n">
-        <v>83.67919921875</v>
+        <v>70.05214691162109</v>
       </c>
       <c r="G176" t="n">
         <v>1</v>
@@ -5115,7 +5115,7 @@
         <v>0</v>
       </c>
       <c r="F205" t="n">
-        <v>25.50435066223145</v>
+        <v>16.72506332397461</v>
       </c>
       <c r="G205" t="n">
         <v>0</v>
@@ -5137,7 +5137,7 @@
         <v>0</v>
       </c>
       <c r="F206" t="n">
-        <v>26.23283863067627</v>
+        <v>18.6953067779541</v>
       </c>
       <c r="G206" t="n">
         <v>0</v>
@@ -5159,7 +5159,7 @@
         <v>0</v>
       </c>
       <c r="F207" t="n">
-        <v>27.53090858459473</v>
+        <v>28.81044149398804</v>
       </c>
       <c r="G207" t="n">
         <v>0</v>
@@ -5181,7 +5181,7 @@
         <v>0</v>
       </c>
       <c r="F208" t="n">
-        <v>34.18350219726562</v>
+        <v>37.89198398590088</v>
       </c>
       <c r="G208" t="n">
         <v>0.5178821879382889</v>
@@ -5203,7 +5203,7 @@
         <v>0</v>
       </c>
       <c r="F209" t="n">
-        <v>40.71933031082153</v>
+        <v>52.61421203613281</v>
       </c>
       <c r="G209" t="n">
         <v>0.9214901477832512</v>
@@ -5225,7 +5225,7 @@
         <v>0</v>
       </c>
       <c r="F210" t="n">
-        <v>83.58218669891349</v>
+        <v>222.1382975578305</v>
       </c>
       <c r="G210" t="n">
         <v>1</v>
@@ -5247,7 +5247,7 @@
         <v>0</v>
       </c>
       <c r="F211" t="n">
-        <v>117.4447536468506</v>
+        <v>349.463939666748</v>
       </c>
       <c r="G211" t="n">
         <v>1</v>
@@ -5931,7 +5931,7 @@
         <v>0</v>
       </c>
       <c r="F241" t="n">
-        <v>0</v>
+        <v>3.598880767822266</v>
       </c>
       <c r="G241" t="n">
         <v>0</v>
@@ -5953,7 +5953,7 @@
         <v>0</v>
       </c>
       <c r="F242" t="n">
-        <v>0</v>
+        <v>8.295178413391113</v>
       </c>
       <c r="G242" t="n">
         <v>0</v>
@@ -5975,7 +5975,7 @@
         <v>0</v>
       </c>
       <c r="F243" t="n">
-        <v>3.392338752746582</v>
+        <v>9.53376293182373</v>
       </c>
       <c r="G243" t="n">
         <v>0</v>
@@ -5997,7 +5997,7 @@
         <v>0</v>
       </c>
       <c r="F244" t="n">
-        <v>8.514583110809326</v>
+        <v>10.05858182907104</v>
       </c>
       <c r="G244" t="n">
         <v>0</v>
@@ -6019,7 +6019,7 @@
         <v>0</v>
       </c>
       <c r="F245" t="n">
-        <v>14.04286623001098</v>
+        <v>15.08040428161621</v>
       </c>
       <c r="G245" t="n">
         <v>0.6620689655172407</v>
@@ -6041,7 +6041,7 @@
         <v>0</v>
       </c>
       <c r="F246" t="n">
-        <v>16.53313636779785</v>
+        <v>15.7923698425293</v>
       </c>
       <c r="G246" t="n">
         <v>0.9310344827586207</v>
@@ -6703,7 +6703,7 @@
         <v>0</v>
       </c>
       <c r="F275" t="n">
-        <v>3.041982650756836</v>
+        <v>4.53639030456543</v>
       </c>
       <c r="G275" t="n">
         <v>0</v>
@@ -6725,7 +6725,7 @@
         <v>0</v>
       </c>
       <c r="F276" t="n">
-        <v>4.270327091217041</v>
+        <v>6.079626083374023</v>
       </c>
       <c r="G276" t="n">
         <v>0</v>
@@ -6747,7 +6747,7 @@
         <v>0</v>
       </c>
       <c r="F277" t="n">
-        <v>6.913959980010986</v>
+        <v>8.040904998779297</v>
       </c>
       <c r="G277" t="n">
         <v>0</v>
@@ -6769,7 +6769,7 @@
         <v>0</v>
       </c>
       <c r="F278" t="n">
-        <v>8.066177368164062</v>
+        <v>9.339213371276855</v>
       </c>
       <c r="G278" t="n">
         <v>0</v>
@@ -6791,7 +6791,7 @@
         <v>0</v>
       </c>
       <c r="F279" t="n">
-        <v>13.71598243713379</v>
+        <v>14.96833562850952</v>
       </c>
       <c r="G279" t="n">
         <v>0</v>
@@ -6813,7 +6813,7 @@
         <v>0</v>
       </c>
       <c r="F280" t="n">
-        <v>15.43868780136108</v>
+        <v>18.06657314300537</v>
       </c>
       <c r="G280" t="n">
         <v>0.01896551724137927</v>
@@ -6835,7 +6835,7 @@
         <v>0</v>
       </c>
       <c r="F281" t="n">
-        <v>16.50309562683105</v>
+        <v>19.02937889099121</v>
       </c>
       <c r="G281" t="n">
         <v>0.03448275862068965</v>
@@ -7497,7 +7497,7 @@
         <v>0</v>
       </c>
       <c r="F310" t="n">
-        <v>48.31337928771973</v>
+        <v>40.66205024719238</v>
       </c>
       <c r="G310" t="n">
         <v>0</v>
@@ -7519,7 +7519,7 @@
         <v>0</v>
       </c>
       <c r="F311" t="n">
-        <v>48.81527423858643</v>
+        <v>43.96588802337646</v>
       </c>
       <c r="G311" t="n">
         <v>0</v>
@@ -7541,7 +7541,7 @@
         <v>0</v>
       </c>
       <c r="F312" t="n">
-        <v>52.18678712844849</v>
+        <v>59.2692494392395</v>
       </c>
       <c r="G312" t="n">
         <v>0.5489130434782609</v>
@@ -7563,7 +7563,7 @@
         <v>0</v>
       </c>
       <c r="F313" t="n">
-        <v>64.13483619689941</v>
+        <v>74.21457767486572</v>
       </c>
       <c r="G313" t="n">
         <v>0.75</v>
@@ -7585,7 +7585,7 @@
         <v>0</v>
       </c>
       <c r="F314" t="n">
-        <v>65.22417068481445</v>
+        <v>88.94813060760498</v>
       </c>
       <c r="G314" t="n">
         <v>0.79047976011994</v>
@@ -7607,7 +7607,7 @@
         <v>0</v>
       </c>
       <c r="F315" t="n">
-        <v>82.15154409408566</v>
+        <v>146.2499022483825</v>
       </c>
       <c r="G315" t="n">
         <v>0.9024193548387096</v>
@@ -7629,7 +7629,7 @@
         <v>0</v>
       </c>
       <c r="F316" t="n">
-        <v>93.98770332336426</v>
+        <v>170.6409454345703</v>
       </c>
       <c r="G316" t="n">
         <v>0.9545454545454546</v>
@@ -8291,7 +8291,7 @@
         <v>0</v>
       </c>
       <c r="F345" t="n">
-        <v>0</v>
+        <v>5.041599273681641</v>
       </c>
       <c r="G345" t="n">
         <v>0</v>
@@ -8313,7 +8313,7 @@
         <v>0</v>
       </c>
       <c r="F346" t="n">
-        <v>0</v>
+        <v>5.772662162780762</v>
       </c>
       <c r="G346" t="n">
         <v>0</v>
@@ -8335,7 +8335,7 @@
         <v>0</v>
       </c>
       <c r="F347" t="n">
-        <v>6.017386913299561</v>
+        <v>7.713854312896729</v>
       </c>
       <c r="G347" t="n">
         <v>0.6092980295566502</v>
@@ -8357,7 +8357,7 @@
         <v>0</v>
       </c>
       <c r="F348" t="n">
-        <v>7.344603538513184</v>
+        <v>7.993698120117188</v>
       </c>
       <c r="G348" t="n">
         <v>0.875</v>
@@ -8379,7 +8379,7 @@
         <v>0</v>
       </c>
       <c r="F349" t="n">
-        <v>10.81645488739014</v>
+        <v>9.370386600494385</v>
       </c>
       <c r="G349" t="n">
         <v>1</v>
@@ -8401,7 +8401,7 @@
         <v>0</v>
       </c>
       <c r="F350" t="n">
-        <v>15.88191986083984</v>
+        <v>16.01730585098267</v>
       </c>
       <c r="G350" t="n">
         <v>1</v>
@@ -8423,7 +8423,7 @@
         <v>0</v>
       </c>
       <c r="F351" t="n">
-        <v>16.01195335388184</v>
+        <v>16.48926734924316</v>
       </c>
       <c r="G351" t="n">
         <v>1</v>
@@ -9129,7 +9129,7 @@
         <v>0</v>
       </c>
       <c r="F382" t="n">
-        <v>4.061579704284668</v>
+        <v>3.662526607513428</v>
       </c>
       <c r="G382" t="n">
         <v>0</v>
@@ -9151,7 +9151,7 @@
         <v>0</v>
       </c>
       <c r="F383" t="n">
-        <v>6.874799728393555</v>
+        <v>8.046388626098633</v>
       </c>
       <c r="G383" t="n">
         <v>0</v>
@@ -9173,7 +9173,7 @@
         <v>0</v>
       </c>
       <c r="F384" t="n">
-        <v>9.878933429718018</v>
+        <v>8.676350116729736</v>
       </c>
       <c r="G384" t="n">
         <v>0</v>
@@ -9195,7 +9195,7 @@
         <v>0</v>
       </c>
       <c r="F385" t="n">
-        <v>11.10649108886719</v>
+        <v>10.00897884368896</v>
       </c>
       <c r="G385" t="n">
         <v>0.9624999999999999</v>
@@ -9217,7 +9217,7 @@
         <v>0</v>
       </c>
       <c r="F386" t="n">
-        <v>11.70730590820312</v>
+        <v>10.29586791992188</v>
       </c>
       <c r="G386" t="n">
         <v>1</v>
@@ -9901,7 +9901,7 @@
         <v>0</v>
       </c>
       <c r="F416" t="n">
-        <v>10.65577268600464</v>
+        <v>12.79209852218628</v>
       </c>
       <c r="G416" t="n">
         <v>0</v>
@@ -9923,7 +9923,7 @@
         <v>0</v>
       </c>
       <c r="F417" t="n">
-        <v>24.97708797454834</v>
+        <v>31.01474046707153</v>
       </c>
       <c r="G417" t="n">
         <v>0</v>
@@ -9945,7 +9945,7 @@
         <v>0</v>
       </c>
       <c r="F418" t="n">
-        <v>34.10398960113525</v>
+        <v>39.22808170318604</v>
       </c>
       <c r="G418" t="n">
         <v>0.6304347826086957</v>
@@ -9967,7 +9967,7 @@
         <v>0</v>
       </c>
       <c r="F419" t="n">
-        <v>121.3383674621582</v>
+        <v>72.36778736114502</v>
       </c>
       <c r="G419" t="n">
         <v>0.9596774193548387</v>
@@ -9989,7 +9989,7 @@
         <v>0.5499999999999989</v>
       </c>
       <c r="F420" t="n">
-        <v>287.0335340499876</v>
+        <v>191.738224029541</v>
       </c>
       <c r="G420" t="n">
         <v>1</v>
@@ -10011,7 +10011,7 @@
         <v>1</v>
       </c>
       <c r="F421" t="n">
-        <v>350.6896495819092</v>
+        <v>219.0546989440918</v>
       </c>
       <c r="G421" t="n">
         <v>1</v>
@@ -10673,7 +10673,7 @@
         <v>0</v>
       </c>
       <c r="F450" t="n">
-        <v>20.4460620880127</v>
+        <v>22.91059494018555</v>
       </c>
       <c r="G450" t="n">
         <v>0</v>
@@ -10695,7 +10695,7 @@
         <v>0</v>
       </c>
       <c r="F451" t="n">
-        <v>22.09926843643188</v>
+        <v>22.94224500656128</v>
       </c>
       <c r="G451" t="n">
         <v>0</v>
@@ -10717,7 +10717,7 @@
         <v>0</v>
       </c>
       <c r="F452" t="n">
-        <v>26.49319171905518</v>
+        <v>27.09120512008667</v>
       </c>
       <c r="G452" t="n">
         <v>0</v>
@@ -10739,7 +10739,7 @@
         <v>0</v>
       </c>
       <c r="F453" t="n">
-        <v>31.16965293884277</v>
+        <v>36.63945198059082</v>
       </c>
       <c r="G453" t="n">
         <v>0.5</v>
@@ -10761,7 +10761,7 @@
         <v>0</v>
       </c>
       <c r="F454" t="n">
-        <v>44.08711194992065</v>
+        <v>50.99308490753174</v>
       </c>
       <c r="G454" t="n">
         <v>1</v>
@@ -10783,7 +10783,7 @@
         <v>0</v>
       </c>
       <c r="F455" t="n">
-        <v>131.7822337150572</v>
+        <v>190.881597995758</v>
       </c>
       <c r="G455" t="n">
         <v>1</v>
@@ -10805,7 +10805,7 @@
         <v>0</v>
       </c>
       <c r="F456" t="n">
-        <v>193.5701370239258</v>
+        <v>207.3073387145996</v>
       </c>
       <c r="G456" t="n">
         <v>1</v>
@@ -11467,7 +11467,7 @@
         <v>0</v>
       </c>
       <c r="F485" t="n">
-        <v>16.03507995605469</v>
+        <v>12.30263710021973</v>
       </c>
       <c r="G485" t="n">
         <v>0</v>
@@ -11489,7 +11489,7 @@
         <v>0</v>
       </c>
       <c r="F486" t="n">
-        <v>16.03572368621826</v>
+        <v>13.17306756973267</v>
       </c>
       <c r="G486" t="n">
         <v>0</v>
@@ -11511,7 +11511,7 @@
         <v>0</v>
       </c>
       <c r="F487" t="n">
-        <v>16.51632785797119</v>
+        <v>21.68565988540649</v>
       </c>
       <c r="G487" t="n">
         <v>0.96777950310559</v>
@@ -11533,7 +11533,7 @@
         <v>0</v>
       </c>
       <c r="F488" t="n">
-        <v>22.40443229675293</v>
+        <v>23.93829822540283</v>
       </c>
       <c r="G488" t="n">
         <v>1</v>
@@ -11555,7 +11555,7 @@
         <v>0</v>
       </c>
       <c r="F489" t="n">
-        <v>24.31690692901611</v>
+        <v>25.16293525695801</v>
       </c>
       <c r="G489" t="n">
         <v>1</v>
@@ -11577,7 +11577,7 @@
         <v>0</v>
       </c>
       <c r="F490" t="n">
-        <v>62.5585556030273</v>
+        <v>30.24462461471557</v>
       </c>
       <c r="G490" t="n">
         <v>1</v>
@@ -11599,7 +11599,7 @@
         <v>0</v>
       </c>
       <c r="F491" t="n">
-        <v>80.49845695495605</v>
+        <v>32.64284133911133</v>
       </c>
       <c r="G491" t="n">
         <v>1</v>
@@ -12261,7 +12261,7 @@
         <v>0</v>
       </c>
       <c r="F520" t="n">
-        <v>65.94133377075195</v>
+        <v>102.527379989624</v>
       </c>
       <c r="G520" t="n">
         <v>0</v>
@@ -12283,7 +12283,7 @@
         <v>0</v>
       </c>
       <c r="F521" t="n">
-        <v>66.07834100723267</v>
+        <v>107.3583602905273</v>
       </c>
       <c r="G521" t="n">
         <v>0</v>
@@ -12305,7 +12305,7 @@
         <v>0</v>
       </c>
       <c r="F522" t="n">
-        <v>66.73687696456909</v>
+        <v>119.4368004798889</v>
       </c>
       <c r="G522" t="n">
         <v>0.9288793103448276</v>
@@ -12327,7 +12327,7 @@
         <v>0</v>
       </c>
       <c r="F523" t="n">
-        <v>81.46262168884277</v>
+        <v>137.0326280593872</v>
       </c>
       <c r="G523" t="n">
         <v>1</v>
@@ -12349,7 +12349,7 @@
         <v>0</v>
       </c>
       <c r="F524" t="n">
-        <v>115.2452230453491</v>
+        <v>177.2399544715881</v>
       </c>
       <c r="G524" t="n">
         <v>1</v>
@@ -12371,7 +12371,7 @@
         <v>0</v>
       </c>
       <c r="F525" t="n">
-        <v>231.198227405548</v>
+        <v>250.5567669868469</v>
       </c>
       <c r="G525" t="n">
         <v>1</v>
@@ -12393,7 +12393,7 @@
         <v>0</v>
       </c>
       <c r="F526" t="n">
-        <v>293.9643859863281</v>
+        <v>253.9701461791992</v>
       </c>
       <c r="G526" t="n">
         <v>1</v>
@@ -13055,7 +13055,7 @@
         <v>0</v>
       </c>
       <c r="F555" t="n">
-        <v>509.9363327026367</v>
+        <v>653.5487174987793</v>
       </c>
       <c r="G555" t="n">
         <v>0</v>
@@ -13077,7 +13077,7 @@
         <v>0</v>
       </c>
       <c r="F556" t="n">
-        <v>516.2836194038391</v>
+        <v>680.7798981666565</v>
       </c>
       <c r="G556" t="n">
         <v>0</v>
@@ -13099,7 +13099,7 @@
         <v>0</v>
       </c>
       <c r="F557" t="n">
-        <v>560.4355931282043</v>
+        <v>776.4614224433899</v>
       </c>
       <c r="G557" t="n">
         <v>0.7760093167701864</v>
@@ -13121,7 +13121,7 @@
         <v>0</v>
       </c>
       <c r="F558" t="n">
-        <v>620.0437545776367</v>
+        <v>918.9643859863281</v>
       </c>
       <c r="G558" t="n">
         <v>0.8297101449275363</v>
@@ -13143,7 +13143,7 @@
         <v>0</v>
       </c>
       <c r="F559" t="n">
-        <v>711.2365961074829</v>
+        <v>1015.517115592957</v>
       </c>
       <c r="G559" t="n">
         <v>0.892741935483871</v>
@@ -13165,7 +13165,7 @@
         <v>0</v>
       </c>
       <c r="F560" t="n">
-        <v>735.5216860771179</v>
+        <v>1063.24657201767</v>
       </c>
       <c r="G560" t="n">
         <v>0.9795454545454545</v>
@@ -13187,7 +13187,7 @@
         <v>0</v>
       </c>
       <c r="F561" t="n">
-        <v>744.3516254425049</v>
+        <v>1097.378969192505</v>
       </c>
       <c r="G561" t="n">
         <v>1</v>

</xml_diff>